<commit_message>
Added the batch integration tests
</commit_message>
<xml_diff>
--- a/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
+++ b/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Folio\mod-rs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F79C76E-C3B0-40FB-91A4-C824CCA65417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B19967-0B7E-4398-B11F-9696E3B53833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="4155" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="195" yWindow="4860" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="138">
   <si>
     <t>Controller</t>
   </si>
@@ -628,7 +628,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -659,8 +659,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -885,8 +883,8 @@
   </sheetPr>
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -981,35 +979,45 @@
       <c r="B11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="3"/>
+      <c r="C12" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
@@ -1055,16 +1063,16 @@
       <c r="B21" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="30" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1079,14 +1087,14 @@
       <c r="A24" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="28" t="s">
         <v>97</v>
       </c>
       <c r="C24" s="13"/>
     </row>
     <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="19" t="s">
         <v>98</v>
       </c>
       <c r="C25" s="3"/>
@@ -1117,7 +1125,7 @@
       <c r="B29" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="31" t="s">
+      <c r="C29" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1126,7 +1134,7 @@
       <c r="B30" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="33" t="s">
+      <c r="C30" s="31" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1211,7 +1219,7 @@
       <c r="B41" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="31" t="s">
+      <c r="C41" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1220,7 +1228,7 @@
       <c r="B42" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="31" t="s">
+      <c r="C42" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1326,7 +1334,7 @@
       <c r="B56" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="32" t="s">
+      <c r="C56" s="30" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1335,7 +1343,7 @@
       <c r="B57" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C57" s="31" t="s">
+      <c r="C57" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1358,7 +1366,7 @@
       <c r="B60" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="C60" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1374,7 +1382,7 @@
       <c r="B62" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="C62" s="31" t="s">
+      <c r="C62" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1392,7 +1400,7 @@
       <c r="B64" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="31" t="s">
+      <c r="C64" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1461,7 +1469,7 @@
       <c r="B73" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="C73" s="31" t="s">
+      <c r="C73" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1545,7 +1553,7 @@
       <c r="B83" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C83" s="31" t="s">
+      <c r="C83" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1554,7 +1562,7 @@
       <c r="B84" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C84" s="31" t="s">
+      <c r="C84" s="29" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1667,7 +1675,7 @@
       <c r="B99" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C99" s="33" t="s">
+      <c r="C99" s="31" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1678,7 +1686,7 @@
       <c r="B100" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C100" s="33" t="s">
+      <c r="C100" s="31" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the HostLMS tests
</commit_message>
<xml_diff>
--- a/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
+++ b/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Folio\mod-rs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B19967-0B7E-4398-B11F-9696E3B53833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D42B99-DB53-482B-AABB-4E2D10A3C529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="4860" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="4770" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="138">
   <si>
     <t>Controller</t>
   </si>
@@ -503,7 +503,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -533,29 +533,13 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -564,27 +548,278 @@
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="hair">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top style="medium">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
@@ -592,35 +827,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
+      <top style="hair">
+        <color auto="1"/>
       </top>
       <bottom style="medium">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -628,41 +860,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -883,8 +1129,8 @@
   </sheetPr>
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -895,10 +1141,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -906,879 +1152,905 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="7"/>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="14"/>
     </row>
     <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="8"/>
-      <c r="B4" s="19" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="15"/>
     </row>
     <row r="5" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="8"/>
-      <c r="B5" s="19" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="22"/>
+      <c r="C5" s="15"/>
     </row>
     <row r="6" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="8"/>
-      <c r="B6" s="19" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="22"/>
+      <c r="C6" s="15"/>
     </row>
     <row r="7" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="8"/>
-      <c r="B7" s="19" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="15"/>
     </row>
     <row r="8" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="8"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="16"/>
     </row>
     <row r="9" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="8"/>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="7"/>
-      <c r="B10" s="4" t="s">
+      <c r="C9" s="16"/>
+    </row>
+    <row r="10" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="19"/>
     </row>
     <row r="11" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="8"/>
-      <c r="B12" s="2" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8"/>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
-      <c r="B14" s="2" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="16"/>
+      <c r="C16" s="21"/>
     </row>
     <row r="17" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="8"/>
-      <c r="B17" s="19" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="3"/>
+      <c r="C17" s="16"/>
     </row>
     <row r="18" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
-      <c r="B18" s="19" t="s">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="C19" s="3"/>
+      <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="21" t="s">
+      <c r="A20" s="17"/>
+      <c r="B20" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="19"/>
     </row>
     <row r="21" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="C21" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="19" t="s">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C22" s="29" t="s">
+      <c r="C22" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="18" t="s">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="C23" s="17"/>
+      <c r="C23" s="27"/>
     </row>
     <row r="24" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C24" s="13"/>
+      <c r="C24" s="30"/>
     </row>
     <row r="25" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="19" t="s">
+      <c r="A25" s="31"/>
+      <c r="B25" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="33"/>
     </row>
     <row r="26" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="19" t="s">
+      <c r="A26" s="31"/>
+      <c r="B26" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="33"/>
     </row>
     <row r="27" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="19" t="s">
+      <c r="A27" s="31"/>
+      <c r="B27" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="33"/>
     </row>
     <row r="28" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="19" t="s">
+      <c r="A28" s="31"/>
+      <c r="B28" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="33"/>
     </row>
     <row r="29" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="19" t="s">
+      <c r="A29" s="31"/>
+      <c r="B29" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="34" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="35"/>
+      <c r="B30" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="37" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
+      <c r="A31" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="3"/>
+      <c r="C31" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="2" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="3"/>
+      <c r="C32" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="2" t="s">
+      <c r="A33" s="9"/>
+      <c r="B33" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="2" t="s">
+      <c r="A34" s="9"/>
+      <c r="B34" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="7"/>
-      <c r="B35" s="4" t="s">
+      <c r="C34" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="17"/>
+      <c r="B35" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="5"/>
+      <c r="C35" s="19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="3"/>
+      <c r="C36" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="2" t="s">
+      <c r="A37" s="9"/>
+      <c r="B37" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C37" s="3"/>
+      <c r="C37" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="38" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="2" t="s">
+      <c r="A38" s="9"/>
+      <c r="B38" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C38" s="3"/>
+      <c r="C38" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A39" s="8"/>
-      <c r="B39" s="2" t="s">
+      <c r="A39" s="9"/>
+      <c r="B39" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="7"/>
-      <c r="B40" s="6" t="s">
+      <c r="C39" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="5"/>
+      <c r="C40" s="19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
+      <c r="A41" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="8"/>
-      <c r="B42" s="2" t="s">
+      <c r="A42" s="9"/>
+      <c r="B42" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="8"/>
-      <c r="B43" s="2" t="s">
+      <c r="A43" s="9"/>
+      <c r="B43" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="3"/>
+      <c r="C43" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="44" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="8"/>
-      <c r="B44" s="2" t="s">
+      <c r="A44" s="9"/>
+      <c r="B44" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C44" s="3"/>
+      <c r="C44" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="45" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="4" t="s">
+      <c r="A45" s="17"/>
+      <c r="B45" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C45" s="5"/>
+      <c r="C45" s="19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="46" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="16"/>
+      <c r="C46" s="21"/>
     </row>
     <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="8"/>
-      <c r="B47" s="19" t="s">
+      <c r="A47" s="9"/>
+      <c r="B47" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C47" s="3"/>
+      <c r="C47" s="16"/>
     </row>
     <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="8"/>
-      <c r="B48" s="19" t="s">
+      <c r="A48" s="9"/>
+      <c r="B48" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C48" s="3"/>
+      <c r="C48" s="16"/>
     </row>
     <row r="49" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A49" s="8"/>
-      <c r="B49" s="19" t="s">
+      <c r="A49" s="9"/>
+      <c r="B49" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C49" s="3"/>
+      <c r="C49" s="16"/>
     </row>
     <row r="50" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="21" t="s">
+      <c r="A50" s="17"/>
+      <c r="B50" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="5"/>
+      <c r="C50" s="19"/>
     </row>
     <row r="51" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="C51" s="16"/>
+      <c r="C51" s="21"/>
     </row>
     <row r="52" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="8"/>
-      <c r="B52" s="19" t="s">
+      <c r="A52" s="9"/>
+      <c r="B52" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C52" s="3"/>
+      <c r="C52" s="16"/>
     </row>
     <row r="53" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A53" s="8"/>
-      <c r="B53" s="19" t="s">
+      <c r="A53" s="9"/>
+      <c r="B53" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="3"/>
+      <c r="C53" s="16"/>
     </row>
     <row r="54" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A54" s="8"/>
-      <c r="B54" s="19" t="s">
+      <c r="A54" s="9"/>
+      <c r="B54" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C54" s="3"/>
+      <c r="C54" s="16"/>
     </row>
     <row r="55" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="19" t="s">
+      <c r="A55" s="17"/>
+      <c r="B55" s="22" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="3"/>
+      <c r="C55" s="19"/>
     </row>
     <row r="56" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C56" s="30" t="s">
+      <c r="C56" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A57" s="8"/>
-      <c r="B57" s="2" t="s">
+      <c r="A57" s="9"/>
+      <c r="B57" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C57" s="29" t="s">
+      <c r="C57" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A58" s="8"/>
-      <c r="B58" s="2" t="s">
+      <c r="A58" s="9"/>
+      <c r="B58" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C58" s="3"/>
+      <c r="C58" s="16"/>
     </row>
     <row r="59" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A59" s="8"/>
-      <c r="B59" s="2" t="s">
+      <c r="A59" s="9"/>
+      <c r="B59" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C59" s="3"/>
+      <c r="C59" s="16"/>
     </row>
     <row r="60" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A60" s="8"/>
-      <c r="B60" s="2" t="s">
+      <c r="A60" s="9"/>
+      <c r="B60" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C60" s="29" t="s">
+      <c r="C60" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A61" s="8"/>
-      <c r="B61" t="s">
+      <c r="A61" s="9"/>
+      <c r="B61" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C61" s="3"/>
+      <c r="C61" s="16"/>
     </row>
     <row r="62" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A62" s="8"/>
-      <c r="B62" s="19" t="s">
+      <c r="A62" s="9"/>
+      <c r="B62" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C62" s="29" t="s">
+      <c r="C62" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="8"/>
-      <c r="B63" s="2" t="s">
+      <c r="A63" s="9"/>
+      <c r="B63" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="8"/>
-      <c r="B64" s="2" t="s">
+      <c r="A64" s="9"/>
+      <c r="B64" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A65" s="8"/>
-      <c r="B65" s="2" t="s">
+      <c r="A65" s="9"/>
+      <c r="B65" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="C65" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A66" s="8"/>
-      <c r="B66" s="2" t="s">
+      <c r="A66" s="9"/>
+      <c r="B66" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C66" s="3"/>
-    </row>
-    <row r="67" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A67" s="7"/>
-      <c r="B67" s="4" t="s">
+      <c r="C66" s="16"/>
+    </row>
+    <row r="67" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="17"/>
+      <c r="B67" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C67" s="5"/>
+      <c r="C67" s="19"/>
     </row>
     <row r="68" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="B68" s="19" t="s">
+      <c r="B68" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="C68" s="3"/>
+      <c r="C68" s="21"/>
     </row>
     <row r="69" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A69" s="8"/>
-      <c r="B69" s="19" t="s">
+      <c r="A69" s="9"/>
+      <c r="B69" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="C69" s="3"/>
+      <c r="C69" s="16"/>
     </row>
     <row r="70" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A70" s="8"/>
-      <c r="B70" s="19" t="s">
+      <c r="A70" s="9"/>
+      <c r="B70" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C70" s="3"/>
+      <c r="C70" s="16"/>
     </row>
     <row r="71" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="8"/>
-      <c r="B71" s="19" t="s">
+      <c r="A71" s="9"/>
+      <c r="B71" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="C71" s="3"/>
+      <c r="C71" s="16"/>
     </row>
     <row r="72" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="8"/>
-      <c r="B72" s="19" t="s">
+      <c r="A72" s="9"/>
+      <c r="B72" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C72" s="3"/>
+      <c r="C72" s="16"/>
     </row>
     <row r="73" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="8"/>
-      <c r="B73" s="19" t="s">
+      <c r="A73" s="9"/>
+      <c r="B73" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C73" s="29" t="s">
+      <c r="C73" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A74" s="8"/>
-      <c r="B74" s="2" t="s">
+      <c r="A74" s="9"/>
+      <c r="B74" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C74" s="3"/>
+      <c r="C74" s="16"/>
     </row>
     <row r="75" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
-      <c r="B75" s="4" t="s">
+      <c r="A75" s="17"/>
+      <c r="B75" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C75" s="5"/>
-    </row>
-    <row r="76" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
+      <c r="C75" s="19"/>
+    </row>
+    <row r="76" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C76" s="5"/>
-    </row>
-    <row r="77" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A77" s="7" t="s">
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C77" s="5"/>
+      <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C78" s="3" t="s">
+      <c r="C78" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A79" s="8"/>
-      <c r="B79" s="2" t="s">
+      <c r="A79" s="9"/>
+      <c r="B79" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C79" s="3"/>
+      <c r="C79" s="16"/>
     </row>
     <row r="80" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A80" s="8"/>
-      <c r="B80" s="2" t="s">
+      <c r="A80" s="9"/>
+      <c r="B80" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C80" s="3"/>
+      <c r="C80" s="16"/>
     </row>
     <row r="81" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A81" s="8"/>
-      <c r="B81" s="2" t="s">
+      <c r="A81" s="9"/>
+      <c r="B81" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C81" s="3" t="s">
+      <c r="C81" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
-      <c r="B82" s="4" t="s">
+      <c r="A82" s="17"/>
+      <c r="B82" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="C82" s="5"/>
+      <c r="C82" s="19"/>
     </row>
     <row r="83" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A83" s="8" t="s">
+      <c r="A83" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C83" s="29" t="s">
+      <c r="C83" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A84" s="8"/>
-      <c r="B84" s="2" t="s">
+      <c r="A84" s="9"/>
+      <c r="B84" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C84" s="29" t="s">
+      <c r="C84" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A85" s="8"/>
-      <c r="B85" s="2" t="s">
+      <c r="A85" s="9"/>
+      <c r="B85" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C85" s="3"/>
+      <c r="C85" s="16"/>
     </row>
     <row r="86" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A86" s="8"/>
-      <c r="B86" s="2" t="s">
+      <c r="A86" s="9"/>
+      <c r="B86" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C86" s="3"/>
+      <c r="C86" s="16"/>
     </row>
     <row r="87" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
-      <c r="B87" s="4" t="s">
+      <c r="A87" s="17"/>
+      <c r="B87" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C87" s="5"/>
+      <c r="C87" s="19"/>
     </row>
     <row r="88" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A88" s="15" t="s">
+      <c r="A88" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="C88" s="16"/>
+      <c r="C88" s="21"/>
     </row>
     <row r="89" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A89" s="8"/>
-      <c r="B89" s="19" t="s">
+      <c r="A89" s="9"/>
+      <c r="B89" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="C89" s="3"/>
+      <c r="C89" s="16"/>
     </row>
     <row r="90" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A90" s="8"/>
-      <c r="B90" s="19" t="s">
+      <c r="A90" s="9"/>
+      <c r="B90" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="C90" s="3"/>
+      <c r="C90" s="16"/>
     </row>
     <row r="91" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A91" s="8"/>
-      <c r="B91" s="19" t="s">
+      <c r="A91" s="9"/>
+      <c r="B91" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="C91" s="3"/>
+      <c r="C91" s="16"/>
     </row>
     <row r="92" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="7"/>
-      <c r="B92" s="21" t="s">
+      <c r="A92" s="17"/>
+      <c r="B92" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="C92" s="5"/>
+      <c r="C92" s="19"/>
     </row>
     <row r="93" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A93" s="15" t="s">
+      <c r="A93" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B93" s="19" t="s">
+      <c r="B93" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C93" s="16"/>
+      <c r="C93" s="21"/>
     </row>
     <row r="94" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A94" s="8"/>
-      <c r="B94" s="19" t="s">
+      <c r="A94" s="9"/>
+      <c r="B94" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C94" s="3"/>
+      <c r="C94" s="16"/>
     </row>
     <row r="95" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="8"/>
-      <c r="B95" s="19" t="s">
+      <c r="A95" s="9"/>
+      <c r="B95" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C95" s="3"/>
+      <c r="C95" s="16"/>
     </row>
     <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A96" s="8"/>
-      <c r="B96" s="19" t="s">
+      <c r="A96" s="9"/>
+      <c r="B96" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C96" s="3"/>
+      <c r="C96" s="16"/>
     </row>
     <row r="97" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="7"/>
-      <c r="B97" s="21" t="s">
+      <c r="A97" s="17"/>
+      <c r="B97" s="22" t="s">
         <v>130</v>
       </c>
-      <c r="C97" s="5"/>
+      <c r="C97" s="19"/>
     </row>
     <row r="98" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A98" s="15" t="s">
+      <c r="A98" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="B98" s="27" t="s">
+      <c r="B98" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C98" s="16"/>
+      <c r="C98" s="21"/>
     </row>
     <row r="99" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="7"/>
-      <c r="B99" s="4" t="s">
+      <c r="A99" s="17"/>
+      <c r="B99" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C99" s="31" t="s">
+      <c r="C99" s="41" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="7" t="s">
+      <c r="A100" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C100" s="31" t="s">
+      <c r="C100" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A101" s="15" t="s">
+      <c r="A101" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B101" s="19" t="s">
+      <c r="B101" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="C101" s="16"/>
+      <c r="C101" s="21"/>
     </row>
     <row r="102" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="7"/>
-      <c r="B102" s="19" t="s">
+      <c r="A102" s="17"/>
+      <c r="B102" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="C102" s="5"/>
+      <c r="C102" s="19"/>
     </row>
     <row r="103" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A103" s="15" t="s">
+      <c r="A103" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B103" s="20" t="s">
+      <c r="B103" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C103" s="16"/>
+      <c r="C103" s="21"/>
     </row>
     <row r="104" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A104" s="8"/>
-      <c r="B104" s="19" t="s">
+      <c r="A104" s="9"/>
+      <c r="B104" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C104" s="3"/>
+      <c r="C104" s="16"/>
     </row>
     <row r="105" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A105" s="8"/>
-      <c r="B105" s="19" t="s">
+      <c r="A105" s="9"/>
+      <c r="B105" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="C105" s="3"/>
+      <c r="C105" s="16"/>
     </row>
     <row r="106" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A106" s="8"/>
-      <c r="B106" s="19" t="s">
+      <c r="A106" s="9"/>
+      <c r="B106" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="C106" s="3"/>
+      <c r="C106" s="16"/>
     </row>
     <row r="107" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="10"/>
-      <c r="B107" s="18" t="s">
+      <c r="A107" s="25"/>
+      <c r="B107" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C107" s="17"/>
+      <c r="C107" s="27"/>
     </row>
     <row r="108" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A108" s="11" t="s">
+      <c r="A108" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B108" s="12" t="s">
+      <c r="B108" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="C108" s="13"/>
+      <c r="C108" s="30"/>
     </row>
     <row r="109" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A109" s="9"/>
-      <c r="B109" s="19" t="s">
+      <c r="A109" s="43"/>
+      <c r="B109" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C109" s="3"/>
+      <c r="C109" s="33"/>
     </row>
     <row r="110" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A110" s="9"/>
-      <c r="B110" s="2" t="s">
+      <c r="A110" s="43"/>
+      <c r="B110" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="C110" s="3"/>
+      <c r="C110" s="33"/>
     </row>
     <row r="111" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A111" s="9"/>
-      <c r="B111" s="2" t="s">
+      <c r="A111" s="43"/>
+      <c r="B111" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="C111" s="3"/>
-    </row>
-    <row r="112" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A112" s="7"/>
-      <c r="B112" s="4" t="s">
+      <c r="C111" s="33"/>
+    </row>
+    <row r="112" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="35"/>
+      <c r="B112" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C112" s="5"/>
+      <c r="C112" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added tests for ShelvingLocation, NoticePolicy, ShelvingLocationSite and Timer
</commit_message>
<xml_diff>
--- a/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
+++ b/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Folio\mod-rs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D42B99-DB53-482B-AABB-4E2D10A3C529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E54F6B-FE81-4595-9FCF-B038C38C7560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="4770" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="4695" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="134">
   <si>
     <t>Controller</t>
   </si>
@@ -358,21 +358,6 @@
     <t>DELETE noticePolicies/{id}</t>
   </si>
   <si>
-    <t>GET patron/$patronIdentifier</t>
-  </si>
-  <si>
-    <t>GET patron</t>
-  </si>
-  <si>
-    <t>POST patron</t>
-  </si>
-  <si>
-    <t>PUT patron/{id}</t>
-  </si>
-  <si>
-    <t>DELETE patron/{id}</t>
-  </si>
-  <si>
     <t>Application</t>
   </si>
   <si>
@@ -434,6 +419,9 @@
   </si>
   <si>
     <t>End Points</t>
+  </si>
+  <si>
+    <t>GET patron/$patronIdentifier/canCreateRequest</t>
   </si>
 </sst>
 </file>
@@ -1127,10 +1115,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1145,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1153,10 +1141,10 @@
     </row>
     <row r="2" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C2" s="7"/>
     </row>
@@ -1307,7 +1295,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C21" s="23" t="s">
         <v>45</v>
@@ -1316,7 +1304,7 @@
     <row r="22" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="10" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C22" s="24" t="s">
         <v>45</v>
@@ -1325,7 +1313,7 @@
     <row r="23" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="26" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C23" s="27"/>
     </row>
@@ -1532,111 +1520,127 @@
       <c r="B46" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="21"/>
+      <c r="C46" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="47" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
       <c r="B47" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="C47" s="16"/>
+      <c r="C47" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
       <c r="B48" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C48" s="16"/>
+      <c r="C48" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="9"/>
       <c r="B49" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C49" s="16"/>
+      <c r="C49" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="50" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17"/>
       <c r="B50" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="19"/>
-    </row>
-    <row r="51" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="C50" s="19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
       <c r="C51" s="21"/>
     </row>
     <row r="52" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="9"/>
-      <c r="B52" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="C52" s="16"/>
+      <c r="A52" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="23" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="53" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
-      <c r="B53" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C53" s="16"/>
+      <c r="B53" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="24" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="54" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="9"/>
-      <c r="B54" s="10" t="s">
-        <v>115</v>
+      <c r="B54" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="C54" s="16"/>
     </row>
-    <row r="55" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17"/>
-      <c r="B55" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C55" s="19"/>
+    <row r="55" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A55" s="9"/>
+      <c r="B55" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="16"/>
     </row>
     <row r="56" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A56" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B56" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="C56" s="23" t="s">
+      <c r="A56" s="9"/>
+      <c r="B56" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56" s="24" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="9"/>
-      <c r="B57" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>45</v>
-      </c>
+      <c r="B57" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C57" s="16"/>
     </row>
     <row r="58" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="9"/>
-      <c r="B58" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C58" s="16"/>
+      <c r="B58" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C58" s="24" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="59" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="9"/>
       <c r="B59" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="C59" s="16"/>
+        <v>44</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="60" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="9"/>
       <c r="B60" s="11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C60" s="24" t="s">
         <v>45</v>
@@ -1644,168 +1648,172 @@
     </row>
     <row r="61" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="9"/>
-      <c r="B61" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="C61" s="16"/>
+      <c r="B61" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="62" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="9"/>
-      <c r="B62" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C62" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A63" s="9"/>
-      <c r="B63" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C63" s="16" t="s">
-        <v>45</v>
-      </c>
+      <c r="B62" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" s="16"/>
+    </row>
+    <row r="63" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="17"/>
+      <c r="B63" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" s="19"/>
     </row>
     <row r="64" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A64" s="9"/>
-      <c r="B64" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C64" s="24" t="s">
-        <v>45</v>
-      </c>
+      <c r="A64" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C64" s="21"/>
     </row>
     <row r="65" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="9"/>
-      <c r="B65" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="C65" s="16" t="s">
-        <v>45</v>
-      </c>
+      <c r="B65" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="16"/>
     </row>
     <row r="66" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="9"/>
-      <c r="B66" s="11" t="s">
-        <v>48</v>
+      <c r="B66" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="C66" s="16"/>
     </row>
-    <row r="67" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="17"/>
-      <c r="B67" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="C67" s="19"/>
+    <row r="67" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A67" s="9"/>
+      <c r="B67" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="16"/>
     </row>
     <row r="68" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A68" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C68" s="21"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="16"/>
     </row>
     <row r="69" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="9"/>
       <c r="B69" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="C69" s="16"/>
+        <v>51</v>
+      </c>
+      <c r="C69" s="24" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="70" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="9"/>
-      <c r="B70" s="10" t="s">
-        <v>89</v>
+      <c r="B70" s="11" t="s">
+        <v>52</v>
       </c>
       <c r="C70" s="16"/>
     </row>
-    <row r="71" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A71" s="9"/>
-      <c r="B71" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="C71" s="16"/>
-    </row>
-    <row r="72" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A72" s="9"/>
-      <c r="B72" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="C72" s="16"/>
-    </row>
-    <row r="73" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A73" s="9"/>
-      <c r="B73" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C73" s="24" t="s">
-        <v>45</v>
-      </c>
+    <row r="71" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="17"/>
+      <c r="B71" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C71" s="19"/>
+    </row>
+    <row r="72" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C73" s="3"/>
     </row>
     <row r="74" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A74" s="9"/>
-      <c r="B74" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C74" s="16"/>
-    </row>
-    <row r="75" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="17"/>
-      <c r="B75" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C75" s="19"/>
-    </row>
-    <row r="76" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C76" s="3"/>
+      <c r="A74" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B74" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C74" s="21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="9"/>
+      <c r="B75" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C75" s="16"/>
+    </row>
+    <row r="76" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A76" s="9"/>
+      <c r="B76" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="77" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C77" s="3"/>
+      <c r="A77" s="17"/>
+      <c r="B77" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C77" s="19"/>
     </row>
     <row r="78" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C78" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C78" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="9"/>
       <c r="B79" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C79" s="16"/>
+        <v>63</v>
+      </c>
+      <c r="C79" s="24" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="80" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="9"/>
       <c r="B80" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="C80" s="16"/>
+        <v>64</v>
+      </c>
+      <c r="C80" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="81" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="9"/>
       <c r="B81" s="11" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="C81" s="16" t="s">
         <v>45</v>
@@ -1814,54 +1822,62 @@
     <row r="82" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="17"/>
       <c r="B82" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C82" s="19"/>
+        <v>66</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="83" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B83" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C83" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C83" s="21" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="9"/>
-      <c r="B84" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C84" s="24" t="s">
+      <c r="B84" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C84" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="9"/>
-      <c r="B85" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C85" s="16"/>
+      <c r="B85" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C85" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="9"/>
-      <c r="B86" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C86" s="16"/>
+      <c r="B86" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C86" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="87" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="17"/>
-      <c r="B87" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C87" s="19"/>
+      <c r="B87" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="C87" s="19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="88" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B88" s="13" t="s">
         <v>121</v>
@@ -1898,159 +1914,132 @@
     </row>
     <row r="93" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B93" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B93" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C93" s="21"/>
+    </row>
+    <row r="94" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="17"/>
+      <c r="B94" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C94" s="41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C95" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A96" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B96" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C93" s="21"/>
-    </row>
-    <row r="94" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A94" s="9"/>
-      <c r="B94" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="C94" s="16"/>
-    </row>
-    <row r="95" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A95" s="9"/>
-      <c r="B95" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="C95" s="16"/>
-    </row>
-    <row r="96" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A96" s="9"/>
-      <c r="B96" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="C96" s="16"/>
+      <c r="C96" s="21"/>
     </row>
     <row r="97" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="17"/>
       <c r="B97" s="22" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C97" s="19"/>
     </row>
     <row r="98" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B98" s="20" t="s">
-        <v>70</v>
+        <v>75</v>
+      </c>
+      <c r="B98" s="13" t="s">
+        <v>86</v>
       </c>
       <c r="C98" s="21"/>
     </row>
-    <row r="99" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="17"/>
-      <c r="B99" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C99" s="41" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C100" s="8" t="s">
-        <v>45</v>
-      </c>
+    <row r="99" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A99" s="9"/>
+      <c r="B99" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C99" s="16"/>
+    </row>
+    <row r="100" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A100" s="9"/>
+      <c r="B100" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C100" s="16"/>
     </row>
     <row r="101" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A101" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="B101" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="C101" s="21"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C101" s="16"/>
     </row>
     <row r="102" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="17"/>
-      <c r="B102" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="C102" s="19"/>
+      <c r="A102" s="25"/>
+      <c r="B102" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C102" s="27"/>
     </row>
     <row r="103" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A103" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B103" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C103" s="21"/>
+      <c r="A103" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B103" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="C103" s="30" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="104" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A104" s="9"/>
-      <c r="B104" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="C104" s="16"/>
+      <c r="A104" s="43"/>
+      <c r="B104" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C104" s="33" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="105" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A105" s="9"/>
-      <c r="B105" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C105" s="16"/>
+      <c r="A105" s="43"/>
+      <c r="B105" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C105" s="33" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="106" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A106" s="9"/>
-      <c r="B106" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C106" s="16"/>
+      <c r="A106" s="43"/>
+      <c r="B106" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C106" s="33" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="107" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="25"/>
-      <c r="B107" s="26" t="s">
-        <v>76</v>
-      </c>
-      <c r="C107" s="27"/>
-    </row>
-    <row r="108" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A108" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B108" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C108" s="30"/>
-    </row>
-    <row r="109" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A109" s="43"/>
-      <c r="B109" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="C109" s="33"/>
-    </row>
-    <row r="110" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A110" s="43"/>
-      <c r="B110" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="C110" s="33"/>
-    </row>
-    <row r="111" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A111" s="43"/>
-      <c r="B111" s="44" t="s">
-        <v>81</v>
-      </c>
-      <c r="C111" s="33"/>
-    </row>
-    <row r="112" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="35"/>
-      <c r="B112" s="36" t="s">
+      <c r="A107" s="35"/>
+      <c r="B107" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="C112" s="45"/>
+      <c r="C107" s="45" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added tests for status
</commit_message>
<xml_diff>
--- a/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
+++ b/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Folio\mod-rs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E54F6B-FE81-4595-9FCF-B038C38C7560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16647094-08AE-4C67-B5CE-3F69564FD56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1125" yWindow="4695" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="134">
   <si>
     <t>Controller</t>
   </si>
@@ -1117,8 +1117,8 @@
   </sheetPr>
   <dimension ref="A1:C107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C98" sqref="C98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1948,14 +1948,18 @@
       <c r="B96" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="C96" s="21"/>
+      <c r="C96" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="97" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A97" s="17"/>
       <c r="B97" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="C97" s="19"/>
+      <c r="C97" s="19" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="98" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="12" t="s">

</xml_diff>

<commit_message>
Tests for Application, App Settings and available action
</commit_message>
<xml_diff>
--- a/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
+++ b/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Folio\mod-rs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D2038E-3E19-40F2-8A4F-9F2CC5BFDC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ABB35D-6609-4985-8EA0-F00FEAFF4ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1620" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="120">
   <si>
     <t>Controller</t>
   </si>
@@ -1100,8 +1100,8 @@
   </sheetPr>
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1129,7 +1129,9 @@
       <c r="B2" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C2" s="6"/>
+      <c r="C2" s="6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
@@ -1138,14 +1140,18 @@
       <c r="B3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
@@ -1653,14 +1659,18 @@
       <c r="B60" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C60" s="46"/>
+      <c r="C60" s="46" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="61" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="8"/>
       <c r="B61" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C61" s="13"/>
+      <c r="C61" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="62" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
@@ -1676,7 +1686,9 @@
       <c r="B63" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="16"/>
+      <c r="C63" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="64" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">

</xml_diff>

<commit_message>
Added tests for template container and fixed typo
</commit_message>
<xml_diff>
--- a/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
+++ b/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Folio\mod-rs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ABB35D-6609-4985-8EA0-F00FEAFF4ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3125B0-4692-43A0-B7C0-D16F073A4D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1620" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="120">
   <si>
     <t>Controller</t>
   </si>
@@ -1100,8 +1100,8 @@
   </sheetPr>
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1877,35 +1877,45 @@
       <c r="B84" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C84" s="18"/>
+      <c r="C84" s="18" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="85" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="8"/>
       <c r="B85" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="13"/>
+      <c r="C85" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="86" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="8"/>
       <c r="B86" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="13"/>
+      <c r="C86" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="87" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="8"/>
       <c r="B87" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="13"/>
+      <c r="C87" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="88" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="22"/>
       <c r="B88" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="C88" s="24"/>
+      <c r="C88" s="24" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="89" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="25" t="s">

</xml_diff>

<commit_message>
Added tests for Shipment and moved the FileDefinition tests into their own file
</commit_message>
<xml_diff>
--- a/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
+++ b/doc/Mod-RS Swagger and Integration Test Coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Source\Folio\mod-rs\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3125B0-4692-43A0-B7C0-D16F073A4D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F0F0AD-BE99-4C8D-BD8B-27CA1774C1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1620" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="1230" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="120">
   <si>
     <t>Controller</t>
   </si>
@@ -1100,8 +1100,8 @@
   </sheetPr>
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1791,35 +1791,45 @@
       <c r="B74" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C74" s="18"/>
+      <c r="C74" s="18" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="75" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="8"/>
       <c r="B75" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C75" s="13"/>
+      <c r="C75" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="76" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="B76" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C76" s="13"/>
+      <c r="C76" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="77" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="8"/>
       <c r="B77" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C77" s="13"/>
+      <c r="C77" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="78" spans="1:3" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="14"/>
       <c r="B78" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="C78" s="16"/>
+      <c r="C78" s="16" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="79" spans="1:3" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="11" t="s">

</xml_diff>